<commit_message>
Commit para reflejar los cambios del día 23 de marzo
</commit_message>
<xml_diff>
--- a/1º Iteración/Grupo Implementación/Tareas Mario.xlsx
+++ b/1º Iteración/Grupo Implementación/Tareas Mario.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TAREAS MARIO OROZCO BORREGO</t>
   </si>
@@ -55,13 +55,34 @@
   </si>
   <si>
     <t>DÍA</t>
+  </si>
+  <si>
+    <t>Modelado del panel Datos Voluntario</t>
+  </si>
+  <si>
+    <t>Modelado del panel Contabilidad</t>
+  </si>
+  <si>
+    <t>NOTAS</t>
+  </si>
+  <si>
+    <t>Tanto tiempo es debido a la primera toma de contacto con el constructor de interfaces, además para adaptarme al estilo definido en los bocetos de interfaz</t>
+  </si>
+  <si>
+    <t>Horas de trabajo</t>
+  </si>
+  <si>
+    <t>Implementacion de la clase ControladorContabilidad, además de la reestructuración de las clases que enlazarían con la vista de Contabilidad. Se han ordenado los listeners de la vista principal de forma que ahora se sabe a qué panel pertenece cada listener</t>
+  </si>
+  <si>
+    <t>Implementacion de la clase ControladorDatosVoluntario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,12 +106,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -99,6 +114,24 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -137,19 +170,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,165 +523,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="1" max="1" width="139.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
     <col min="3" max="3" width="88.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="131" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="128" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28">
+    <row r="1" spans="1:4" ht="28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="23">
+    <row r="4" spans="1:4" ht="23">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5">
+      <c r="B5" s="4">
         <v>40977</v>
       </c>
-      <c r="E5" s="4">
+      <c r="C5" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5">
+      <c r="B6" s="4">
         <v>40978</v>
       </c>
-      <c r="E6" s="4">
+      <c r="C6" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5">
+      <c r="B7" s="4">
         <v>40978</v>
       </c>
-      <c r="E7" s="4">
+      <c r="C7" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5">
+      <c r="B8" s="4">
         <v>40981</v>
       </c>
-      <c r="E8" s="4">
+      <c r="C8" s="3">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5">
+      <c r="B9" s="4">
         <v>40983</v>
       </c>
-      <c r="E9" s="4">
+      <c r="C9" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5">
+      <c r="B10" s="4">
         <v>40989</v>
       </c>
-      <c r="E10" s="4">
+      <c r="C10" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="20">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>40990</v>
+      </c>
+      <c r="C11" s="3">
+        <v>180</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4">
+        <v>40990</v>
+      </c>
+      <c r="C12" s="3">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>40990</v>
+      </c>
+      <c r="C13" s="3">
+        <v>90</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>40990</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" ht="20">
+      <c r="B25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="4">
-        <f>SUM(E5:E14)</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="C25" s="3">
+        <f>SUM(C5:C21)</f>
+        <v>825</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <f>C25/60</f>
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Commit para reflejar los cambios producidos en Dropbox a día 25 de marzo
</commit_message>
<xml_diff>
--- a/1º Iteración/Grupo Implementación/Tareas Mario.xlsx
+++ b/1º Iteración/Grupo Implementación/Tareas Mario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="25600" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="0" windowWidth="24020" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>TAREAS MARIO OROZCO BORREGO</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Comprensión de la arquitectura diseñada por el equipo de implementación de todo el sistema, especialmente de la diseñada para la gestión de la interfaz y sus eventos</t>
   </si>
   <si>
-    <t>DURACION (min)</t>
-  </si>
-  <si>
     <t>TIEMPO TOTAL DE TRABAJO</t>
   </si>
   <si>
@@ -76,6 +73,30 @@
   </si>
   <si>
     <t>Implementacion de la clase ControladorDatosVoluntario</t>
+  </si>
+  <si>
+    <t>Reunión con el equipo de implementación, para tratar aspectos de la arquitectura de la interfaz</t>
+  </si>
+  <si>
+    <t>Reestructuración de la arquitectura de la interfaz</t>
+  </si>
+  <si>
+    <t>Debido a que se hizo sin atender a lo dicho por el grupo de diseño por parte de otro compañero</t>
+  </si>
+  <si>
+    <t>Ajustar ultimos detalles de la reestructuración para poder seguir añadiendo cosas</t>
+  </si>
+  <si>
+    <t>Agregar casi todo lo restante a la interfaz (quedan los Datos Personales de Voluntarios y Beneficiarios, 1 solo panel)</t>
+  </si>
+  <si>
+    <t>Creado el controlador de ayudas y el diseño del panel de datos de beneficiarios</t>
+  </si>
+  <si>
+    <t>Puesta a punto de la interfaz y prueba de los manejadores de eventos de la misma</t>
+  </si>
+  <si>
+    <t>DURACIÓN (min)</t>
   </si>
 </sst>
 </file>
@@ -198,6 +219,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -525,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -549,13 +575,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -632,7 +658,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4">
         <v>40990</v>
@@ -641,12 +667,12 @@
         <v>180</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="4">
         <v>40990</v>
@@ -658,7 +684,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4">
         <v>40990</v>
@@ -670,7 +696,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4">
         <v>40990</v>
@@ -681,39 +707,77 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4">
+        <v>40991</v>
+      </c>
+      <c r="C15" s="3">
+        <v>60</v>
+      </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4">
+        <v>40991</v>
+      </c>
+      <c r="C16" s="3">
+        <v>240</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4">
+        <v>40991</v>
+      </c>
+      <c r="C17" s="3">
+        <v>60</v>
+      </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4">
+        <v>40991</v>
+      </c>
+      <c r="C18" s="3">
+        <v>240</v>
+      </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4">
+        <v>40992</v>
+      </c>
+      <c r="C19" s="3">
+        <v>240</v>
+      </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4">
+        <v>40993</v>
+      </c>
+      <c r="C20" s="3">
+        <v>210</v>
+      </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
@@ -742,21 +806,21 @@
     </row>
     <row r="25" spans="1:4" ht="20">
       <c r="B25" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" s="3">
         <f>SUM(C5:C21)</f>
-        <v>825</v>
+        <v>1875</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="29" spans="1:4">
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
         <f>C25/60</f>
-        <v>13.75</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="30" spans="1:4">

</xml_diff>